<commit_message>
Chagnes for review comments
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -471,7 +471,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,7 +634,7 @@
         <v>22</v>
       </c>
       <c r="I5" s="1">
-        <v>8934346722</v>
+        <v>432434</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>14</v>

</xml_diff>